<commit_message>
some final touchups on testing
</commit_message>
<xml_diff>
--- a/government_shutdown_stats.xlsx
+++ b/government_shutdown_stats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\# Gregs Temp\Rice U DABC\Project 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg_\Data-Bootcamp-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD9A455-A19C-4B2E-9476-BFE650E4FDC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3BD04B6-1DAB-4E31-852D-C19A328A4E89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8865" xr2:uid="{7C7ECD33-EE7F-4020-B0A8-7EC1C6714FF7}"/>
   </bookViews>
@@ -150,9 +150,6 @@
     <t>2018-02-09</t>
   </si>
   <si>
-    <t>Length_in_days</t>
-  </si>
-  <si>
     <t>senate_party_in_power</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>length_in_days</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,16 +557,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,13 +584,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -602,20 +602,20 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D21" si="0">SUM(DATEDIF(MID(B3,6,2)&amp;"/"&amp;MID(B3,9,2)&amp;"/"&amp;MID(B3,1,4),MID(C3,6,2)&amp;"/"&amp;MID(C3,9,2)&amp;"/"&amp;MID(C3,1,4),"D")+1)</f>
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,13 +634,13 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -659,13 +659,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,13 +684,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -709,13 +709,13 @@
         <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -734,13 +734,13 @@
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -759,13 +759,13 @@
         <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -784,13 +784,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -809,13 +809,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -834,13 +834,13 @@
         <v>4</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,13 +859,13 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -884,13 +884,13 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,13 +909,13 @@
         <v>3</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -934,13 +934,13 @@
         <v>5</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,13 +959,13 @@
         <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>33</v>
@@ -984,13 +984,13 @@
         <v>33</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,13 +1009,13 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,13 +1034,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1059,13 +1059,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>